<commit_message>
add new dataset make cv file
</commit_message>
<xml_diff>
--- a/dataset/metadata.xlsx
+++ b/dataset/metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\研究\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\研究\research_b4\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Dataname</t>
     <phoneticPr fontId="1"/>
@@ -99,6 +99,14 @@
   </si>
   <si>
     <t>Australian</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Class ratio</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Satimage</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -174,7 +182,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -185,6 +193,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -481,7 +495,7 @@
     <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,10 +509,10 @@
         <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -515,7 +529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -530,7 +544,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -547,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -564,7 +578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -581,7 +595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -596,7 +610,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -613,7 +627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -630,7 +644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -643,11 +657,43 @@
       <c r="D10">
         <v>11</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E10" s="3">
+        <v>90</v>
+      </c>
+      <c r="F10" s="4">
+        <v>90</v>
+      </c>
+      <c r="G10" s="4">
+        <v>90</v>
+      </c>
+      <c r="H10" s="4">
+        <v>90</v>
+      </c>
+      <c r="I10" s="4">
+        <v>90</v>
+      </c>
+      <c r="J10" s="4">
+        <v>90</v>
+      </c>
+      <c r="K10" s="4">
+        <v>90</v>
+      </c>
+      <c r="L10" s="4">
+        <v>90</v>
+      </c>
+      <c r="M10" s="4">
+        <v>90</v>
+      </c>
+      <c r="N10" s="4">
+        <v>90</v>
+      </c>
+      <c r="O10" s="4">
+        <v>90</v>
+      </c>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -664,7 +710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -681,7 +727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -696,6 +742,38 @@
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="5">
+        <v>6435</v>
+      </c>
+      <c r="C14">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>1533</v>
+      </c>
+      <c r="F14">
+        <v>703</v>
+      </c>
+      <c r="G14">
+        <v>1358</v>
+      </c>
+      <c r="H14">
+        <v>626</v>
+      </c>
+      <c r="I14">
+        <v>707</v>
+      </c>
+      <c r="J14">
+        <v>1508</v>
       </c>
     </row>
   </sheetData>
@@ -704,5 +782,6 @@
   </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify three large datasets
</commit_message>
<xml_diff>
--- a/dataset/metadata.xlsx
+++ b/dataset/metadata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\研究\research_b4\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\y5ule\research\research_b4\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11745" windowHeight="6915"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11748" windowHeight="6912"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Dataname</t>
     <phoneticPr fontId="1"/>
@@ -103,13 +103,25 @@
   </si>
   <si>
     <t>Satimage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Shuttle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Penbased</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Magic</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,21 +492,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -528,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -543,7 +555,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -575,7 +587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -595,7 +607,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -618,7 +630,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -633,7 +645,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -653,7 +665,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -679,7 +691,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -728,7 +740,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -751,7 +763,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -768,7 +780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -785,7 +797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -815,6 +827,105 @@
       </c>
       <c r="J14">
         <v>1508</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="5">
+        <v>57999</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>45586</v>
+      </c>
+      <c r="F15">
+        <v>49</v>
+      </c>
+      <c r="G15">
+        <v>171</v>
+      </c>
+      <c r="H15">
+        <v>8903</v>
+      </c>
+      <c r="I15">
+        <v>3267</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5">
+        <v>10992</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>1143</v>
+      </c>
+      <c r="F16">
+        <v>1143</v>
+      </c>
+      <c r="G16">
+        <v>1144</v>
+      </c>
+      <c r="H16">
+        <v>1055</v>
+      </c>
+      <c r="I16">
+        <v>1144</v>
+      </c>
+      <c r="J16">
+        <v>1055</v>
+      </c>
+      <c r="K16">
+        <v>1056</v>
+      </c>
+      <c r="L16">
+        <v>1142</v>
+      </c>
+      <c r="M16">
+        <v>1055</v>
+      </c>
+      <c r="N16">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5">
+        <v>19020</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>12332</v>
+      </c>
+      <c r="F17">
+        <v>6688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>